<commit_message>
added Custom Weighted Model to combat class imbalance, added differencial loss callback to stop when overfitting, added 2-step classification
</commit_message>
<xml_diff>
--- a/ACL_Experiments.xlsx
+++ b/ACL_Experiments.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\UNAM\2024-II\ACL_classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524277CE-0987-476B-B8E6-461DF9ED2078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD66864-84F4-45AA-A49A-CD53EED5AEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8CC0603E-86A4-4318-A513-182A2CD04AB4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{8CC0603E-86A4-4318-A513-182A2CD04AB4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="SingleClassification" sheetId="1" r:id="rId1"/>
+    <sheet name="DoubleClassification" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="153">
   <si>
     <t>Experiment 1</t>
   </si>
@@ -441,13 +442,67 @@
   </si>
   <si>
     <t>100 (6 tolerance f1, used 24)</t>
+  </si>
+  <si>
+    <t>Experiment 36</t>
+  </si>
+  <si>
+    <t>Experiment 37</t>
+  </si>
+  <si>
+    <t>XLNet-Large without augmentation!</t>
+  </si>
+  <si>
+    <t>Experiment 38</t>
+  </si>
+  <si>
+    <t>70/30/val_data</t>
+  </si>
+  <si>
+    <t>XLNet-Large with ChatGPT4 augmentation (40 texts per class)</t>
+  </si>
+  <si>
+    <t>Experiment 39</t>
+  </si>
+  <si>
+    <t>XLNet-Large, no augmentation, Using WeightedAutoModel!</t>
+  </si>
+  <si>
+    <t>Overfitting after epoch 16</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>Model 1</t>
+  </si>
+  <si>
+    <t>Model 2</t>
+  </si>
+  <si>
+    <t>XLM-Roberta-Large</t>
+  </si>
+  <si>
+    <t>F1 1st</t>
+  </si>
+  <si>
+    <t>F1 2nd</t>
+  </si>
+  <si>
+    <t>Overall F1</t>
+  </si>
+  <si>
+    <t>Experiment 40</t>
+  </si>
+  <si>
+    <t>XLNet-Large, no augmentation, Using WeightedAutoModel, weight_decay=0.02 instead of 0.01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,6 +543,18 @@
     <font>
       <sz val="10"/>
       <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="6"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -588,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -684,6 +751,15 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -708,14 +784,17 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1051,15 +1130,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A6B6DD-2928-433D-B1D2-6CB06CB7586C}">
-  <dimension ref="A1:AM32"/>
+  <dimension ref="A1:AR32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y24" workbookViewId="0">
-      <selection activeCell="AM28" sqref="AM28"/>
+    <sheetView topLeftCell="AE22" workbookViewId="0">
+      <selection activeCell="AR32" sqref="AR32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:39" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:44" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
@@ -1167,9 +1246,24 @@
       <c r="AM1" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="AN1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>151</v>
+      </c>
     </row>
-    <row r="2" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="33" t="s">
+    <row r="2" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="36" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1280,9 +1374,24 @@
       <c r="AM2" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="AN2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AO2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AP2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AQ2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR2" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="34"/>
+    <row r="3" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="37"/>
       <c r="B3" s="3" t="s">
         <v>25</v>
       </c>
@@ -1391,9 +1500,24 @@
       <c r="AM3" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="AN3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AO3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AP3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AQ3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR3" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="34"/>
+    <row r="4" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="37"/>
       <c r="B4" s="3" t="s">
         <v>26</v>
       </c>
@@ -1502,9 +1626,24 @@
       <c r="AM4" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="AN4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AQ4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR4" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="5" spans="1:39" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="34"/>
+    <row r="5" spans="1:44" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="37"/>
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1613,9 +1752,24 @@
       <c r="AM5" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="AN5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AQ5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR5" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="6" spans="1:39" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="34"/>
+    <row r="6" spans="1:44" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="37"/>
       <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
@@ -1724,9 +1878,24 @@
       <c r="AM6" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="AN6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AO6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR6" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="7" spans="1:39" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="34"/>
+    <row r="7" spans="1:44" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="37"/>
       <c r="B7" s="3" t="s">
         <v>32</v>
       </c>
@@ -1835,9 +2004,24 @@
       <c r="AM7" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="AN7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO7" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="AP7" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ7" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR7" s="30" t="s">
+        <v>139</v>
+      </c>
     </row>
-    <row r="8" spans="1:39" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="35"/>
+    <row r="8" spans="1:44" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="38"/>
       <c r="B8" s="3" t="s">
         <v>38</v>
       </c>
@@ -1946,8 +2130,23 @@
       <c r="AM8" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="AN8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AQ8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR8" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="9" spans="1:39" ht="80.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:44" ht="80.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="24"/>
       <c r="B9" s="3" t="s">
         <v>90</v>
@@ -2061,9 +2260,24 @@
       <c r="AM9" s="30" t="s">
         <v>98</v>
       </c>
+      <c r="AN9" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="AO9" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="AP9" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ9" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="AR9" s="30" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="10" spans="1:39" ht="54" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="36" t="s">
+    <row r="10" spans="1:44" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="39" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -2130,9 +2344,14 @@
       <c r="AK10" s="8"/>
       <c r="AL10" s="8"/>
       <c r="AM10" s="8"/>
+      <c r="AN10" s="8"/>
+      <c r="AO10" s="8"/>
+      <c r="AP10" s="8"/>
+      <c r="AQ10" s="8"/>
+      <c r="AR10" s="8"/>
     </row>
-    <row r="11" spans="1:39" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="37"/>
+    <row r="11" spans="1:44" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="40"/>
       <c r="B11" s="8" t="s">
         <v>47</v>
       </c>
@@ -2241,9 +2460,24 @@
       <c r="AM11" s="11" t="s">
         <v>24</v>
       </c>
+      <c r="AN11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AQ11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR11" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="12" spans="1:39" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="37"/>
+    <row r="12" spans="1:44" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="40"/>
       <c r="B12" s="8" t="s">
         <v>48</v>
       </c>
@@ -2352,9 +2586,24 @@
       <c r="AM12" s="11" t="s">
         <v>24</v>
       </c>
+      <c r="AN12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AQ12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR12" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="13" spans="1:39" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="37"/>
+    <row r="13" spans="1:44" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="40"/>
       <c r="B13" s="8" t="s">
         <v>49</v>
       </c>
@@ -2463,9 +2712,24 @@
       <c r="AM13" s="11" t="s">
         <v>24</v>
       </c>
+      <c r="AN13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AQ13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR13" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="14" spans="1:39" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="37"/>
+    <row r="14" spans="1:44" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="40"/>
       <c r="B14" s="8" t="s">
         <v>50</v>
       </c>
@@ -2529,54 +2793,69 @@
       <c r="X14" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="Y14" s="12" t="s">
-        <v>23</v>
+      <c r="Y14" s="27" t="s">
+        <v>24</v>
       </c>
       <c r="Z14" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AA14" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AB14" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AC14" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AD14" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AE14" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AF14" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AG14" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AH14" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AI14" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AJ14" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AK14" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AL14" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AM14" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="AN14" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO14" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP14" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="AQ14" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR14" s="27" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:39" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="37"/>
+    <row r="15" spans="1:44" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="40"/>
       <c r="B15" s="8" t="s">
         <v>51</v>
       </c>
@@ -2685,9 +2964,24 @@
       <c r="AM15" s="11" t="s">
         <v>24</v>
       </c>
+      <c r="AN15" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO15" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP15" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AQ15" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR15" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="16" spans="1:39" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="37"/>
+    <row r="16" spans="1:44" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="40"/>
       <c r="B16" s="8" t="s">
         <v>52</v>
       </c>
@@ -2751,54 +3045,69 @@
       <c r="X16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="Y16" s="12" t="s">
-        <v>23</v>
+      <c r="Y16" s="27" t="s">
+        <v>24</v>
       </c>
       <c r="Z16" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AA16" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AB16" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AC16" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AD16" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AE16" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AF16" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AG16" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AH16" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AI16" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AJ16" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AK16" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AL16" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AM16" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="AN16" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO16" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP16" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="AQ16" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR16" s="27" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:39" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="37"/>
+    <row r="17" spans="1:44" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="40"/>
       <c r="B17" s="8" t="s">
         <v>53</v>
       </c>
@@ -2862,7 +3171,7 @@
       <c r="X17" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="Y17" s="12" t="s">
+      <c r="Y17" s="44" t="s">
         <v>23</v>
       </c>
       <c r="Z17" s="27" t="s">
@@ -2907,9 +3216,24 @@
       <c r="AM17" s="27" t="s">
         <v>23</v>
       </c>
+      <c r="AN17" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="AO17" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP17" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="AQ17" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR17" s="27" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="18" spans="1:39" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="37"/>
+    <row r="18" spans="1:44" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="40"/>
       <c r="B18" s="8" t="s">
         <v>54</v>
       </c>
@@ -3018,9 +3342,24 @@
       <c r="AM18" s="11" t="s">
         <v>24</v>
       </c>
+      <c r="AN18" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO18" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP18" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AQ18" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR18" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="19" spans="1:39" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="37"/>
+    <row r="19" spans="1:44" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="40"/>
       <c r="B19" s="8" t="s">
         <v>55</v>
       </c>
@@ -3129,9 +3468,24 @@
       <c r="AM19" s="27" t="s">
         <v>23</v>
       </c>
+      <c r="AN19" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="AO19" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP19" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="AQ19" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR19" s="27" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="20" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="37"/>
+    <row r="20" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="40"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -3170,9 +3524,14 @@
       <c r="AK20" s="8"/>
       <c r="AL20" s="8"/>
       <c r="AM20" s="8"/>
+      <c r="AN20" s="8"/>
+      <c r="AO20" s="8"/>
+      <c r="AP20" s="8"/>
+      <c r="AQ20" s="8"/>
+      <c r="AR20" s="8"/>
     </row>
-    <row r="21" spans="1:39" ht="54" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="38"/>
+    <row r="21" spans="1:44" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="41"/>
       <c r="B21" s="7" t="s">
         <v>40</v>
       </c>
@@ -3237,8 +3596,13 @@
       <c r="AK21" s="8"/>
       <c r="AL21" s="8"/>
       <c r="AM21" s="8"/>
+      <c r="AN21" s="8"/>
+      <c r="AO21" s="8"/>
+      <c r="AP21" s="8"/>
+      <c r="AQ21" s="8"/>
+      <c r="AR21" s="8"/>
     </row>
-    <row r="22" spans="1:39" ht="159.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:44" ht="159.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>63</v>
       </c>
@@ -3330,8 +3694,23 @@
       <c r="AM22" s="32" t="s">
         <v>132</v>
       </c>
+      <c r="AN22" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="AO22" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="AP22" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="AQ22" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="AR22" s="32" t="s">
+        <v>152</v>
+      </c>
     </row>
-    <row r="23" spans="1:39" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:44" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="16" t="s">
         <v>71</v>
       </c>
@@ -3441,8 +3820,23 @@
       <c r="AM23" s="20">
         <v>5.0000000000000004E-6</v>
       </c>
+      <c r="AN23" s="20">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="AO23" s="20">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="AP23" s="20">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="AQ23" s="20">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="AR23" s="20">
+        <v>5.0000000000000004E-6</v>
+      </c>
     </row>
-    <row r="24" spans="1:39" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:44" ht="54" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="21"/>
       <c r="B24" s="17" t="s">
         <v>74</v>
@@ -3550,8 +3944,23 @@
       <c r="AM24" s="17" t="s">
         <v>134</v>
       </c>
+      <c r="AN24" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO24" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP24" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ24" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AR24" s="17" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="25" spans="1:39" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:44" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="29" t="s">
         <v>102</v>
       </c>
@@ -3642,30 +4051,45 @@
       <c r="AF25" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="AG25" s="41" t="s">
+      <c r="AG25" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="AH25" s="41" t="s">
+      <c r="AH25" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="AI25" s="41" t="s">
+      <c r="AI25" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="AJ25" s="41" t="s">
+      <c r="AJ25" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="AK25" s="41" t="s">
+      <c r="AK25" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="AL25" s="41" t="s">
+      <c r="AL25" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="AM25" s="43" t="s">
+      <c r="AM25" s="35" t="s">
         <v>103</v>
       </c>
+      <c r="AN25" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="AO25" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="AP25" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="AQ25" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="AR25" s="33" t="s">
+        <v>103</v>
+      </c>
     </row>
-    <row r="26" spans="1:39" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="39" t="s">
+    <row r="26" spans="1:44" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="42" t="s">
         <v>78</v>
       </c>
       <c r="B26" s="17" t="s">
@@ -3736,9 +4160,14 @@
       <c r="AK26" s="17"/>
       <c r="AL26" s="17"/>
       <c r="AM26" s="17"/>
+      <c r="AN26" s="17"/>
+      <c r="AO26" s="17"/>
+      <c r="AP26" s="17"/>
+      <c r="AQ26" s="17"/>
+      <c r="AR26" s="17"/>
     </row>
-    <row r="27" spans="1:39" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="40"/>
+    <row r="27" spans="1:44" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="43"/>
       <c r="B27" s="17" t="s">
         <v>83</v>
       </c>
@@ -3806,11 +4235,14 @@
       <c r="AL27" s="17">
         <v>0.41</v>
       </c>
-      <c r="AM27" s="17">
-        <v>0.5</v>
-      </c>
+      <c r="AM27" s="17"/>
+      <c r="AN27" s="17"/>
+      <c r="AO27" s="17"/>
+      <c r="AP27" s="17"/>
+      <c r="AQ27" s="17"/>
+      <c r="AR27" s="17"/>
     </row>
-    <row r="28" spans="1:39" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:44" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="17" t="s">
         <v>86</v>
@@ -3854,8 +4286,15 @@
       <c r="AK28" s="17"/>
       <c r="AL28" s="17"/>
       <c r="AM28" s="17"/>
+      <c r="AN28" s="17"/>
+      <c r="AO28" s="17"/>
+      <c r="AP28" s="17"/>
+      <c r="AQ28" s="17">
+        <v>0.49</v>
+      </c>
+      <c r="AR28" s="17"/>
     </row>
-    <row r="29" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="17" t="s">
         <v>87</v>
@@ -3899,8 +4338,13 @@
       <c r="AK29" s="17"/>
       <c r="AL29" s="17"/>
       <c r="AM29" s="17"/>
+      <c r="AN29" s="17"/>
+      <c r="AO29" s="17"/>
+      <c r="AP29" s="17"/>
+      <c r="AQ29" s="17"/>
+      <c r="AR29" s="17"/>
     </row>
-    <row r="30" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="17" t="s">
         <v>88</v>
@@ -3959,40 +4403,58 @@
       <c r="AK30" s="17"/>
       <c r="AL30" s="17"/>
       <c r="AM30" s="17"/>
+      <c r="AN30" s="17">
+        <v>0.45</v>
+      </c>
+      <c r="AO30" s="45">
+        <v>0.49</v>
+      </c>
+      <c r="AP30" s="46">
+        <v>0.47</v>
+      </c>
+      <c r="AQ30" s="47">
+        <v>0.54</v>
+      </c>
+      <c r="AR30" s="47"/>
     </row>
-    <row r="31" spans="1:39" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:44" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="AD31" s="42" t="s">
+      <c r="AD31" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="AE31" s="42" t="s">
+      <c r="AE31" s="34" t="s">
         <v>105</v>
       </c>
       <c r="AF31" s="17">
         <v>0.2</v>
       </c>
     </row>
-    <row r="32" spans="1:39" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:44" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>63</v>
       </c>
-      <c r="AG32" s="42" t="s">
+      <c r="AG32" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="AH32" s="42" t="s">
+      <c r="AH32" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="AI32" s="42" t="s">
+      <c r="AI32" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="AJ32" s="42" t="s">
+      <c r="AJ32" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="AM32" s="42" t="s">
+      <c r="AM32" s="34" t="s">
         <v>133</v>
       </c>
+      <c r="AN32" s="34"/>
+      <c r="AQ32" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="AR32" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4002,4 +4464,66 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A842D37-9184-4942-A7F8-E2DF89304F96}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>